<commit_message>
Making a timeline of predictions
</commit_message>
<xml_diff>
--- a/Awards Season Timeline.xlsx
+++ b/Awards Season Timeline.xlsx
@@ -9,12 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1110" yWindow="0" windowWidth="27285" windowHeight="11970" xr2:uid="{024F0286-CFA8-454B-86A5-AC7B9D2BAA97}"/>
+    <workbookView xWindow="2220" yWindow="0" windowWidth="27690" windowHeight="12795" xr2:uid="{A272E83F-3723-4449-AFF3-0705C9E88A4B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027" calcMode="manual"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$J$17</definedName>
+  </definedNames>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,39 +27,102 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="32">
+  <si>
+    <t>RT.All</t>
+  </si>
+  <si>
+    <t>RT.Top</t>
+  </si>
+  <si>
+    <t>AA.Actor</t>
+  </si>
+  <si>
+    <t>AA.ActorSup</t>
+  </si>
+  <si>
+    <t>AA.Actress</t>
+  </si>
+  <si>
+    <t>AA.ActressSup</t>
+  </si>
+  <si>
+    <t>AA.Director</t>
+  </si>
+  <si>
+    <t>AA.Adapt</t>
+  </si>
+  <si>
+    <t>AA.Original</t>
+  </si>
+  <si>
+    <t>Globes.Drama</t>
+  </si>
+  <si>
+    <t>Globes.Comedy</t>
+  </si>
+  <si>
+    <t>CCA</t>
+  </si>
+  <si>
+    <t>SAG</t>
+  </si>
+  <si>
+    <t>BAFTA</t>
+  </si>
+  <si>
+    <t>PGA</t>
+  </si>
+  <si>
+    <t>DGA</t>
+  </si>
+  <si>
+    <t>WGA.Original</t>
+  </si>
+  <si>
+    <t>WGA.Adapted</t>
+  </si>
+  <si>
+    <t>WGA</t>
+  </si>
   <si>
     <t>Date</t>
   </si>
   <si>
+    <t>Rotten Tomatoes</t>
+  </si>
+  <si>
     <t>Award</t>
   </si>
   <si>
+    <t>Nom</t>
+  </si>
+  <si>
     <t>Globes</t>
   </si>
   <si>
-    <t>CCA</t>
-  </si>
-  <si>
-    <t>SAG</t>
-  </si>
-  <si>
-    <t>BAFTA</t>
-  </si>
-  <si>
-    <t>PGA</t>
-  </si>
-  <si>
-    <t>DGA</t>
-  </si>
-  <si>
-    <t>WGA</t>
-  </si>
-  <si>
-    <t>Nom</t>
-  </si>
-  <si>
-    <t>NomAward</t>
+    <t>Oscar</t>
+  </si>
+  <si>
+    <t>Var1</t>
+  </si>
+  <si>
+    <t>Var2</t>
+  </si>
+  <si>
+    <t>Var3</t>
+  </si>
+  <si>
+    <t>Var4</t>
+  </si>
+  <si>
+    <t>Var5</t>
+  </si>
+  <si>
+    <t>Var6</t>
+  </si>
+  <si>
+    <t>Var7</t>
   </si>
 </sst>
 </file>
@@ -72,12 +138,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -92,9 +164,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -408,187 +482,324 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{320BA9D2-4219-4414-9180-3DF3EEF27496}">
-  <dimension ref="A1:C15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{627911C6-8CE3-47F8-B8F4-EFDBD47FA0DD}">
+  <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" customWidth="1"/>
     <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1">
+        <v>40878</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1">
+        <v>43075</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1">
+        <v>43080</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1">
+        <v>43082</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="2">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1">
+        <v>43104</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="2">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1">
+        <v>43105</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0</v>
+      </c>
+      <c r="C8" s="1">
+        <v>43107</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="2">
+        <v>1</v>
+      </c>
+      <c r="C9" s="1">
+        <v>43109</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="2">
+        <v>1</v>
+      </c>
+      <c r="C10" s="1">
+        <v>43110</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="2">
+        <v>0</v>
+      </c>
+      <c r="C11" s="1">
+        <v>43111</v>
+      </c>
+      <c r="D11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="2">
+        <v>0</v>
+      </c>
+      <c r="C12" s="1">
+        <v>43120</v>
+      </c>
+      <c r="D12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2">
+        <v>0</v>
+      </c>
+      <c r="C13" s="1">
+        <v>43121</v>
+      </c>
+      <c r="D13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="2">
+        <v>0</v>
+      </c>
+      <c r="C14" s="1">
+        <v>43123</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="1">
-        <v>43075</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="1">
-        <v>43080</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="F14" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="1">
-        <v>43082</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="G14" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J14" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="1">
-        <v>43104</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="1">
-        <v>43105</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" s="1">
-        <v>43107</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="1">
-        <v>43108</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="1">
-        <v>43110</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10" t="s">
-        <v>1</v>
-      </c>
-      <c r="C10" s="1">
-        <v>43111</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C11" s="1">
-        <v>43120</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>4</v>
-      </c>
-      <c r="B12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C12" s="1">
-        <v>43121</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" t="s">
-        <v>1</v>
-      </c>
-      <c r="C13" s="1">
-        <v>43134</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>8</v>
-      </c>
-      <c r="B14" t="s">
-        <v>1</v>
-      </c>
-      <c r="C14" s="1">
-        <v>43142</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>5</v>
-      </c>
-      <c r="B15" t="s">
-        <v>1</v>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="2">
+        <v>0</v>
       </c>
       <c r="C15" s="1">
+        <v>43133</v>
+      </c>
+      <c r="D15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="2">
+        <v>0</v>
+      </c>
+      <c r="C16" s="1">
+        <v>43141</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="2">
+        <v>0</v>
+      </c>
+      <c r="C17" s="1">
         <v>43149</v>
       </c>
+      <c r="D17" t="s">
+        <v>13</v>
+      </c>
     </row>
   </sheetData>
-  <sortState ref="A2:C15">
-    <sortCondition ref="C1"/>
-  </sortState>
+  <autoFilter ref="A1:J17" xr:uid="{26CF2974-0990-43BB-A765-4B984B440E22}">
+    <sortState ref="A2:J17">
+      <sortCondition ref="C1:C17"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
TimeData function that processes data for whether nom/award has happened
</commit_message>
<xml_diff>
--- a/Awards Season Timeline.xlsx
+++ b/Awards Season Timeline.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="32">
   <si>
     <t>RT.All</t>
   </si>
@@ -101,9 +101,6 @@
     <t>Globes</t>
   </si>
   <si>
-    <t>Oscar</t>
-  </si>
-  <si>
     <t>Var1</t>
   </si>
   <si>
@@ -123,6 +120,9 @@
   </si>
   <si>
     <t>Var7</t>
+  </si>
+  <si>
+    <t>AA</t>
   </si>
 </sst>
 </file>
@@ -483,10 +483,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{627911C6-8CE3-47F8-B8F4-EFDBD47FA0DD}">
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -509,25 +509,25 @@
         <v>19</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" t="s">
         <v>25</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>26</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -719,33 +719,33 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="B14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C14" s="1">
         <v>43123</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E14" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="F14" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="G14" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H14" s="2" t="s">
+      <c r="H14" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I14" s="2" t="s">
+      <c r="I14" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J14" s="2" t="s">
+      <c r="J14" s="3" t="s">
         <v>8</v>
       </c>
     </row>
@@ -780,7 +780,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>13</v>
       </c>
@@ -792,6 +792,38 @@
       </c>
       <c r="D17" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" s="2">
+        <v>0</v>
+      </c>
+      <c r="C18" s="1">
+        <v>43163</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>